<commit_message>
RDCC-2480: adding code changes and unit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/Staff Data Upload.xlsx
+++ b/src/test/resources/Staff Data Upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B1C24C-C2F6-8F4D-94EF-8390D64BD22F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A391FEE7-7D32-0D49-88CE-F8DBD21942EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -28,20 +28,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1205">
   <si>
     <t>Region</t>
   </si>
@@ -3653,6 +3645,12 @@
   </si>
   <si>
     <t>test@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>testt</t>
+  </si>
+  <si>
+    <t>testt@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -7650,8 +7648,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8000,31 +7998,51 @@
       <c r="AD4" s="41"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="1" t="str">
+      <c r="A5" s="41" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
         <f>IF(ISNA(VLOOKUP(D5,Region!$A$2:$B$11,2)),"",VLOOKUP(D5,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="1" t="str">
+        <v>5</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1">
         <f>IF(ISNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="1" t="str">
+        <v>817181</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="1">
         <f>IF(ISNA(VLOOKUP(H5,'Base Locations'!A4:F344,2)),"",VLOOKUP(H5,'Base Locations'!A4:F344,2))</f>
-        <v/>
-      </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+        <v>239985</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>1169</v>
+      </c>
       <c r="N5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BHA3</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="1" t="str">
@@ -8061,8 +8079,12 @@
         <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
+      <c r="AC5" s="41" t="s">
+        <v>1199</v>
+      </c>
+      <c r="AD5" s="41" t="s">
+        <v>1121</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>

</xml_diff>

<commit_message>
RDCC-2480: changed blank row handling logic and updated test files
</commit_message>
<xml_diff>
--- a/src/test/resources/Staff Data Upload.xlsx
+++ b/src/test/resources/Staff Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A391FEE7-7D32-0D49-88CE-F8DBD21942EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F020320-CFD8-1A40-8FAD-1598E531FC5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1203">
   <si>
     <t>Region</t>
   </si>
@@ -3645,12 +3645,6 @@
   </si>
   <si>
     <t>test@justice.gov.uk</t>
-  </si>
-  <si>
-    <t>testt</t>
-  </si>
-  <si>
-    <t>testt@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -7648,7 +7642,7 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
@@ -7998,51 +7992,31 @@
       <c r="AD4" s="41"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>1204</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D5,Region!$A$2:$B$11,2)),"",VLOOKUP(D5,Region!$A$2:$B$11,2))</f>
-        <v>5</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="1">
+        <v/>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F5,'Base Locations'!$A$1:$F$341,2))</f>
-        <v>817181</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" s="1">
+        <v/>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(H5,'Base Locations'!A4:F344,2)),"",VLOOKUP(H5,'Base Locations'!A4:F344,2))</f>
-        <v>239985</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>408</v>
-      </c>
-      <c r="L5" s="41" t="s">
-        <v>409</v>
-      </c>
-      <c r="M5" s="41" t="s">
-        <v>1169</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
       <c r="N5" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M5,Services!$A$1:$B$45,2)),"",VLOOKUP(M5,Services!$A$1:$B$45,2))</f>
-        <v>BHA3</v>
+        <v/>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="1" t="str">
@@ -8079,12 +8053,8 @@
         <f>IF(ISNA(VLOOKUP(AA5,Services!$A$1:$B$45,2)),"",VLOOKUP(AA5,Services!$A$1:$B$45,2))</f>
         <v/>
       </c>
-      <c r="AC5" s="41" t="s">
-        <v>1199</v>
-      </c>
-      <c r="AD5" s="41" t="s">
-        <v>1121</v>
-      </c>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>

</xml_diff>